<commit_message>
Add Cypress for end-to-end testing
</commit_message>
<xml_diff>
--- a/cypress/fixtures/loginData.xlsx
+++ b/cypress/fixtures/loginData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28906"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28914"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bu.shafique\Documents\BankUltimus_Automation\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAB8BCED-453A-48E2-9B54-641DE2B66F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2267E6DD-3E90-4CD0-ADCE-B2A5C698AEE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" firstSheet="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
   <si>
     <t>url</t>
   </si>
@@ -52,7 +52,7 @@
     <t>http://192.168.10.199/BankUltimusSPARK</t>
   </si>
   <si>
-    <t>shafique1</t>
+    <t>shafique2</t>
   </si>
   <si>
     <t>HomePageUrl</t>
@@ -109,6 +109,63 @@
     <t>BirthRegIssDate</t>
   </si>
   <si>
+    <t>PlaceOfBirth</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>IntroducerType</t>
+  </si>
+  <si>
+    <t>AddressType</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>LandPhone</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>CityTownArea</t>
+  </si>
+  <si>
+    <t>ZIP_PostalCode</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Division_State</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>FName</t>
+  </si>
+  <si>
+    <t>MName</t>
+  </si>
+  <si>
+    <t>CustConcentration</t>
+  </si>
+  <si>
+    <t>KYC_Prof</t>
+  </si>
+  <si>
+    <t>KYC_Open_Nature</t>
+  </si>
+  <si>
     <t>Md</t>
   </si>
   <si>
@@ -127,6 +184,9 @@
     <t>1238529051753</t>
   </si>
   <si>
+    <t>7890103564</t>
+  </si>
+  <si>
     <t>B00075189</t>
   </si>
   <si>
@@ -149,6 +209,48 @@
   </si>
   <si>
     <t>11/10/1993</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Service Holder in IT Sector</t>
+  </si>
+  <si>
+    <t>NID Verified</t>
+  </si>
+  <si>
+    <t>Permanent Address</t>
+  </si>
+  <si>
+    <t>College Road Area</t>
+  </si>
+  <si>
+    <t>4566978213</t>
+  </si>
+  <si>
+    <t>01811111112</t>
+  </si>
+  <si>
+    <t>Chashara</t>
+  </si>
+  <si>
+    <t>1230</t>
+  </si>
+  <si>
+    <t>NARAYANGANJ</t>
+  </si>
+  <si>
+    <t>Rashidul Islam</t>
+  </si>
+  <si>
+    <t>Jahan Ara</t>
+  </si>
+  <si>
+    <t>Non-Govt/Private Service Holder</t>
+  </si>
+  <si>
+    <t>Self/Walk-In</t>
   </si>
 </sst>
 </file>
@@ -211,8 +313,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -496,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -547,7 +649,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
@@ -572,124 +674,256 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E5813B1-5843-40D8-80A2-E35B896B6A5A}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AF6" sqref="AF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="17" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="16" style="4" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="16" style="4" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="4" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="4" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="4"/>
-    <col min="14" max="14" width="17.28515625" style="4" customWidth="1"/>
-    <col min="15" max="15" width="26.28515625" style="4" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.5703125" style="3" customWidth="1"/>
+    <col min="22" max="22" width="14.7109375" style="3" customWidth="1"/>
+    <col min="23" max="23" width="16.5703125" style="3" customWidth="1"/>
+    <col min="24" max="24" width="18.140625" style="3" customWidth="1"/>
+    <col min="25" max="25" width="14.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.28515625" style="3" customWidth="1"/>
+    <col min="27" max="27" width="18.28515625" style="3" customWidth="1"/>
+    <col min="28" max="28" width="17.140625" style="3" customWidth="1"/>
+    <col min="29" max="29" width="16.5703125" style="3" customWidth="1"/>
+    <col min="30" max="31" width="9.140625" style="3"/>
+    <col min="32" max="32" width="28.85546875" style="3" customWidth="1"/>
+    <col min="33" max="33" width="24.5703125" style="3" customWidth="1"/>
+    <col min="34" max="34" width="18.7109375" style="3" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:34">
+      <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="P1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="4">
-        <v>7890103564</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>36</v>
+    <row r="2" spans="1:34">
+      <c r="A2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CIF Info Update 127
</commit_message>
<xml_diff>
--- a/cypress/fixtures/loginData.xlsx
+++ b/cypress/fixtures/loginData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28926"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bu.shafique\Documents\BankUltimus_Automation\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C979AA2-28C6-440A-B626-4E4998C9AB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F10354D5-200C-45D3-85F3-22FC350AF82C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="79">
   <si>
     <t>url</t>
   </si>
@@ -122,6 +122,12 @@
     <t>Occupation</t>
   </si>
   <si>
+    <t>MonthlyIncome</t>
+  </si>
+  <si>
+    <t>ResidenceLoc</t>
+  </si>
+  <si>
     <t>IntroducerType</t>
   </si>
   <si>
@@ -155,6 +161,9 @@
     <t>PS</t>
   </si>
   <si>
+    <t>PO</t>
+  </si>
+  <si>
     <t>FName</t>
   </si>
   <si>
@@ -218,7 +227,13 @@
     <t>Male</t>
   </si>
   <si>
-    <t>Service Holder in IT Sector</t>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>70000</t>
+  </si>
+  <si>
+    <t>Resident</t>
   </si>
   <si>
     <t>NID Verified</t>
@@ -236,13 +251,16 @@
     <t>01811111112</t>
   </si>
   <si>
-    <t>Chashara</t>
+    <t>Dhamrai</t>
   </si>
   <si>
     <t>1230</t>
   </si>
   <si>
-    <t>NARAYANGANJ</t>
+    <t>DHAMRAI</t>
+  </si>
+  <si>
+    <t>Dhaka Main PO</t>
   </si>
   <si>
     <t>Khan Mahbub</t>
@@ -251,10 +269,13 @@
     <t>Rahima Begum</t>
   </si>
   <si>
-    <t>Non-Govt/Private Service Holder</t>
-  </si>
-  <si>
-    <t>Self/Walk-In</t>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Service in Information &amp; Technology Sector</t>
+  </si>
+  <si>
+    <t>Walk-in/Unsolicited</t>
   </si>
 </sst>
 </file>
@@ -658,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB203C0-CA1F-4DE4-9DFD-626961E733A7}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -713,10 +734,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E5813B1-5843-40D8-80A2-E35B896B6A5A}">
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AK2" sqref="AK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -739,26 +760,27 @@
     <col min="16" max="16" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.5703125" style="2" customWidth="1"/>
-    <col min="22" max="22" width="14.7109375" style="2" customWidth="1"/>
-    <col min="23" max="23" width="16.5703125" style="2" customWidth="1"/>
-    <col min="24" max="24" width="18.140625" style="2" customWidth="1"/>
-    <col min="25" max="25" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.28515625" style="2" customWidth="1"/>
-    <col min="27" max="27" width="18.28515625" style="2" customWidth="1"/>
-    <col min="28" max="28" width="17.140625" style="2" customWidth="1"/>
-    <col min="29" max="29" width="16.5703125" style="2" customWidth="1"/>
-    <col min="30" max="30" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="28.85546875" style="2" customWidth="1"/>
-    <col min="33" max="33" width="24.5703125" style="2" customWidth="1"/>
-    <col min="34" max="34" width="18.7109375" style="2" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="2"/>
+    <col min="19" max="20" width="24.42578125" style="2" customWidth="1"/>
+    <col min="21" max="21" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.5703125" style="2" customWidth="1"/>
+    <col min="24" max="24" width="14.7109375" style="2" customWidth="1"/>
+    <col min="25" max="25" width="16.5703125" style="2" customWidth="1"/>
+    <col min="26" max="26" width="18.140625" style="2" customWidth="1"/>
+    <col min="27" max="27" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.28515625" style="2" customWidth="1"/>
+    <col min="29" max="29" width="18.28515625" style="2" customWidth="1"/>
+    <col min="30" max="30" width="17.140625" style="2" customWidth="1"/>
+    <col min="31" max="32" width="16.5703125" style="2" customWidth="1"/>
+    <col min="33" max="33" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="28.85546875" style="2" customWidth="1"/>
+    <col min="36" max="36" width="44" style="2" customWidth="1"/>
+    <col min="37" max="37" width="18.7109375" style="2" customWidth="1"/>
+    <col min="38" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:37">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -861,109 +883,127 @@
       <c r="AH1" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="AI1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:37">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="R2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC2" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="AD2" s="2" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK2" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
login data excel with failed message
</commit_message>
<xml_diff>
--- a/cypress/fixtures/loginData.xlsx
+++ b/cypress/fixtures/loginData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bu.shafique\Documents\BankUltimus_Automation\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9F9B77F-98C7-47F5-ACA8-DC1F1F505AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEAA683A-A64A-4E36-BE2F-9CA285E1FF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -182,7 +182,7 @@
     <t>Md</t>
   </si>
   <si>
-    <t>Rony</t>
+    <t>Anthony</t>
   </si>
   <si>
     <t>H.</t>
@@ -194,13 +194,13 @@
     <t>BANGLADESHI</t>
   </si>
   <si>
-    <t>9514931229018</t>
-  </si>
-  <si>
-    <t>9200963821</t>
-  </si>
-  <si>
-    <t>B00229480</t>
+    <t>9414931229018</t>
+  </si>
+  <si>
+    <t>9200963827</t>
+  </si>
+  <si>
+    <t>B00229880</t>
   </si>
   <si>
     <t>21/01/2020</t>
@@ -737,7 +737,7 @@
   <dimension ref="A1:AK2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>